<commit_message>
Backend Added For Marksheet 1
</commit_message>
<xml_diff>
--- a/DATA/Final_format_of_marksheet_1_2_combined.xlsx
+++ b/DATA/Final_format_of_marksheet_1_2_combined.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaibhav\Desktop\Electrocom\marksheet_Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaibhav\Desktop\Electrocom\marksheet\DATA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CDBB74FC-6AE3-40C3-AD1C-154EE6DF1977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB7C94A0-9AFC-4BAD-BA96-657E615123E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2748" windowWidth="17280" windowHeight="8964" xr2:uid="{1D8BFEE0-7E4D-46E3-BC6A-8C8F8972C366}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1D8BFEE0-7E4D-46E3-BC6A-8C8F8972C366}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <t>block</t>
   </si>
   <si>
-    <t>kendra_code</t>
-  </si>
-  <si>
     <t>school_dice_code</t>
   </si>
   <si>
@@ -96,13 +93,16 @@
     <t>environmental_studies</t>
   </si>
   <si>
-    <t>working_education</t>
-  </si>
-  <si>
     <t>physical</t>
   </si>
   <si>
     <t>arts</t>
+  </si>
+  <si>
+    <t>examination_center_code</t>
+  </si>
+  <si>
+    <t>work_education</t>
   </si>
 </sst>
 </file>
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84A9B68D-0373-47E3-A8EB-C778A9E9A060}">
   <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,28 +476,28 @@
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
-      </c>
-      <c r="H1" t="s">
-        <v>12</v>
       </c>
       <c r="I1" t="s">
         <v>0</v>
@@ -509,49 +509,49 @@
         <v>2</v>
       </c>
       <c r="L1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M1" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="N1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>23</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>